<commit_message>
Added use case for edit/update service directory
</commit_message>
<xml_diff>
--- a/Analysis/Test Cases/System Test Case Summary.xlsx
+++ b/Analysis/Test Cases/System Test Case Summary.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="77">
   <si>
     <t>Title</t>
   </si>
@@ -100,9 +100,6 @@
   </si>
   <si>
     <t>Service Management</t>
-  </si>
-  <si>
-    <t>Get all service information</t>
   </si>
   <si>
     <t>Add service record for a member</t>
@@ -263,9 +260,6 @@
     <t>User should be able to delete a provider.</t>
   </si>
   <si>
-    <t>User should be able to get the list of all available services.</t>
-  </si>
-  <si>
     <t>User should be able to add a service record for a member.</t>
   </si>
   <si>
@@ -291,6 +285,24 @@
   </si>
   <si>
     <t>The system should be able to generate weekly EFT data for all providers. The system will generate the data as previously scheduled by a user.</t>
+  </si>
+  <si>
+    <t>Show validation status and go back to menu upon success. And on error return back to menu.</t>
+  </si>
+  <si>
+    <t>SRVM003</t>
+  </si>
+  <si>
+    <t>Edit/update service directory</t>
+  </si>
+  <si>
+    <t>Get all service directory</t>
+  </si>
+  <si>
+    <t>User should be able to update service directory information.</t>
+  </si>
+  <si>
+    <t>User should be able to get the list of all available service directory information.</t>
   </si>
 </sst>
 </file>
@@ -797,9 +809,9 @@
   <dimension ref="A3:H42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -859,7 +871,7 @@
     <row r="7" spans="1:8" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
@@ -868,18 +880,20 @@
         <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="F7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="1"/>
+      <c r="G7" s="1" t="s">
+        <v>71</v>
+      </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>15</v>
@@ -888,10 +902,10 @@
         <v>16</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
@@ -899,7 +913,7 @@
     <row r="9" spans="1:8" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>15</v>
@@ -908,10 +922,10 @@
         <v>18</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -919,7 +933,7 @@
     <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>15</v>
@@ -928,10 +942,10 @@
         <v>19</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -939,7 +953,7 @@
     <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>15</v>
@@ -948,10 +962,10 @@
         <v>20</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
@@ -959,7 +973,7 @@
     <row r="12" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>15</v>
@@ -968,10 +982,10 @@
         <v>21</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
@@ -979,7 +993,7 @@
     <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>15</v>
@@ -988,10 +1002,10 @@
         <v>22</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -999,7 +1013,7 @@
     <row r="14" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>15</v>
@@ -1008,10 +1022,10 @@
         <v>23</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
@@ -1019,7 +1033,7 @@
     <row r="15" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
@@ -1028,10 +1042,10 @@
         <v>24</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -1039,19 +1053,19 @@
     <row r="16" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1059,39 +1073,39 @@
     <row r="17" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>46</v>
+        <v>72</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>29</v>
+        <v>73</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>65</v>
+        <v>75</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
@@ -1099,19 +1113,19 @@
     <row r="19" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C19" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="E19" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
@@ -1119,19 +1133,19 @@
     <row r="20" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1139,16 +1153,16 @@
     <row r="21" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>67</v>
@@ -1159,19 +1173,19 @@
     <row r="22" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>32</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1179,19 +1193,19 @@
     <row r="23" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1199,30 +1213,40 @@
     <row r="24" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>53</v>
-      </c>
       <c r="F24" s="1" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
+      <c r="B25" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F25" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>

</xml_diff>

<commit_message>
Added more use cases
</commit_message>
<xml_diff>
--- a/Analysis/Test Cases/System Test Case Summary.xlsx
+++ b/Analysis/Test Cases/System Test Case Summary.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="86">
   <si>
     <t>Title</t>
   </si>
@@ -303,6 +303,33 @@
   </si>
   <si>
     <t>User should be able to get the list of all available service directory information.</t>
+  </si>
+  <si>
+    <t>SRVM004</t>
+  </si>
+  <si>
+    <t>SRVM005</t>
+  </si>
+  <si>
+    <t>Verify a recorded service</t>
+  </si>
+  <si>
+    <t>User should be able to verify the list of provided service.</t>
+  </si>
+  <si>
+    <t>Verify weeky service fee</t>
+  </si>
+  <si>
+    <t>User should be able to verify the wwekly service fee.</t>
+  </si>
+  <si>
+    <t>ACTM009</t>
+  </si>
+  <si>
+    <t>Update member status</t>
+  </si>
+  <si>
+    <t>User should be able to update member status.</t>
   </si>
 </sst>
 </file>
@@ -1053,19 +1080,19 @@
     <row r="16" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>74</v>
+        <v>84</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1073,19 +1100,19 @@
     <row r="17" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>26</v>
+        <v>74</v>
       </c>
       <c r="E17" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -1093,79 +1120,79 @@
     <row r="18" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>73</v>
+        <v>26</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>45</v>
+        <v>72</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>28</v>
+        <v>73</v>
       </c>
       <c r="E19" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>33</v>
+        <v>79</v>
       </c>
       <c r="E20" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>64</v>
+        <v>80</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>30</v>
+        <v>81</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
@@ -1173,19 +1200,19 @@
     <row r="22" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="E22" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
@@ -1193,19 +1220,19 @@
     <row r="23" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="E23" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
@@ -1213,19 +1240,19 @@
     <row r="24" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>69</v>
+        <v>30</v>
       </c>
       <c r="E24" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
@@ -1233,50 +1260,80 @@
     <row r="25" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="E25" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
+      <c r="B27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>68</v>
+      </c>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A28" s="4"/>
-      <c r="B28" s="4"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
+      <c r="B28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>70</v>
+      </c>
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>

</xml_diff>

<commit_message>
Added SRVM004 detail test file. Renamed SRVM001 detail test file.
</commit_message>
<xml_diff>
--- a/Analysis/Test Cases/System Test Case Summary.xlsx
+++ b/Analysis/Test Cases/System Test Case Summary.xlsx
@@ -314,9 +314,6 @@
     <t>Verify a recorded service</t>
   </si>
   <si>
-    <t>User should be able to verify the list of provided service.</t>
-  </si>
-  <si>
     <t>Verify weeky service fee</t>
   </si>
   <si>
@@ -330,6 +327,9 @@
   </si>
   <si>
     <t>User should be able to update member status.</t>
+  </si>
+  <si>
+    <t>User should be able to verify the list of weekly provided service.</t>
   </si>
 </sst>
 </file>
@@ -835,10 +835,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="F16" sqref="F16"/>
+      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1080,19 +1080,19 @@
     <row r="16" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E16" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -1172,7 +1172,7 @@
         <v>52</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>80</v>
+        <v>85</v>
       </c>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
@@ -1186,13 +1186,13 @@
         <v>25</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E21" s="1" t="s">
         <v>52</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>

</xml_diff>

<commit_message>
Updated the expected results in the Test Case Summary
Updated rows: ACTM003, ACTM008, RPRT004, & SRVM004
</commit_message>
<xml_diff>
--- a/Analysis/Test Cases/System Test Case Summary.xlsx
+++ b/Analysis/Test Cases/System Test Case Summary.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="90">
   <si>
     <t>Title</t>
   </si>
@@ -330,6 +330,18 @@
   </si>
   <si>
     <t>User should be able to verify the list of weekly provided service.</t>
+  </si>
+  <si>
+    <t>Member information is updated in the system. Success message is shown.</t>
+  </si>
+  <si>
+    <t>Provider information is deleted from the system. Success message is shown.</t>
+  </si>
+  <si>
+    <t>The weekly provider report checklist is marked as "verified" in the system. Success message is shown.</t>
+  </si>
+  <si>
+    <t>Weekly provider report scheduler's day and time are changed properly. The reports are generated according to the new schedule. Success message is shown.</t>
   </si>
 </sst>
 </file>
@@ -835,10 +847,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -974,7 +986,9 @@
       <c r="F10" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="G10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
@@ -1074,7 +1088,9 @@
       <c r="F15" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="G15" s="1"/>
+      <c r="G15" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -1174,7 +1190,9 @@
       <c r="F20" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="G20" s="1"/>
+      <c r="G20" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
@@ -1274,7 +1292,9 @@
       <c r="F25" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="G25" s="1"/>
+      <c r="G25" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
@@ -1334,8 +1354,8 @@
       <c r="F28" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A29" s="4"/>

</xml_diff>

<commit_message>
Changes due to meeting updates
</commit_message>
<xml_diff>
--- a/Analysis/Test Cases/System Test Case Summary.xlsx
+++ b/Analysis/Test Cases/System Test Case Summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7670" tabRatio="900"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7665" tabRatio="900"/>
   </bookViews>
   <sheets>
     <sheet name="Authentication" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="91">
   <si>
     <t>Title</t>
   </si>
@@ -342,6 +342,9 @@
   </si>
   <si>
     <t>Weekly provider report scheduler's day and time are changed properly. The reports are generated according to the new schedule. Success message is shown.</t>
+  </si>
+  <si>
+    <t>Show member information</t>
   </si>
 </sst>
 </file>
@@ -847,32 +850,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
+      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.26953125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="2"/>
+    <col min="3" max="3" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E3" s="10" t="s">
         <v>12</v>
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>11</v>
       </c>
@@ -881,7 +884,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>7</v>
       </c>
@@ -907,7 +910,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
         <v>34</v>
@@ -929,7 +932,7 @@
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
         <v>35</v>
@@ -946,10 +949,12 @@
       <c r="F8" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="G8" s="1"/>
+      <c r="G8" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
         <v>36</v>
@@ -969,7 +974,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
         <v>37</v>
@@ -991,7 +996,7 @@
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
         <v>38</v>
@@ -1011,7 +1016,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
         <v>39</v>
@@ -1031,7 +1036,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
         <v>40</v>
@@ -1051,7 +1056,7 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
         <v>41</v>
@@ -1071,7 +1076,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
         <v>42</v>
@@ -1093,7 +1098,7 @@
       </c>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
         <v>82</v>
@@ -1113,7 +1118,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
         <v>44</v>
@@ -1133,7 +1138,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
         <v>43</v>
@@ -1153,7 +1158,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
         <v>72</v>
@@ -1173,7 +1178,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
         <v>77</v>
@@ -1195,7 +1200,7 @@
       </c>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
         <v>78</v>
@@ -1215,7 +1220,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
         <v>45</v>
@@ -1235,7 +1240,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
         <v>46</v>
@@ -1255,7 +1260,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
         <v>47</v>
@@ -1275,7 +1280,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
         <v>48</v>
@@ -1297,7 +1302,7 @@
       </c>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>49</v>
@@ -1317,7 +1322,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1" t="s">
         <v>50</v>
@@ -1337,7 +1342,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="1" t="s">
         <v>51</v>
@@ -1357,7 +1362,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1367,7 +1372,7 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1377,7 +1382,7 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1387,7 +1392,7 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1397,7 +1402,7 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1407,7 +1412,7 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1417,7 +1422,7 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1427,7 +1432,7 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1437,7 +1442,7 @@
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1447,7 +1452,7 @@
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1457,7 +1462,7 @@
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1467,7 +1472,7 @@
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1477,7 +1482,7 @@
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1487,7 +1492,7 @@
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1518,20 +1523,20 @@
       <selection pane="bottomLeft" activeCell="C2" sqref="C2:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.26953125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="2"/>
+    <col min="3" max="3" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -1557,7 +1562,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1571,7 +1576,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1581,7 +1586,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1591,7 +1596,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1601,7 +1606,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1611,7 +1616,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -1621,7 +1626,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1631,7 +1636,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1641,7 +1646,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1651,7 +1656,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1661,7 +1666,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1671,7 +1676,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1681,7 +1686,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1691,7 +1696,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1701,7 +1706,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1711,7 +1716,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1721,7 +1726,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1731,7 +1736,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1741,7 +1746,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1751,7 +1756,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1761,7 +1766,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1771,7 +1776,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1781,7 +1786,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1791,7 +1796,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1801,7 +1806,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1811,7 +1816,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1821,7 +1826,7 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1831,7 +1836,7 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1841,7 +1846,7 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1851,7 +1856,7 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1861,7 +1866,7 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1871,7 +1876,7 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1881,7 +1886,7 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1891,7 +1896,7 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1901,7 +1906,7 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1911,7 +1916,7 @@
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1937,20 +1942,20 @@
       <selection pane="bottomLeft" activeCell="C2" sqref="C2:H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.26953125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="2"/>
+    <col min="3" max="3" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -1976,7 +1981,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
@@ -1990,7 +1995,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2000,7 +2005,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -2010,7 +2015,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -2020,7 +2025,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2030,7 +2035,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
@@ -2040,7 +2045,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2050,7 +2055,7 @@
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -2060,7 +2065,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2070,7 +2075,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2080,7 +2085,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2090,7 +2095,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -2100,7 +2105,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2110,7 +2115,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -2120,7 +2125,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -2130,7 +2135,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -2140,7 +2145,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -2150,7 +2155,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -2160,7 +2165,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -2170,7 +2175,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -2180,7 +2185,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -2190,7 +2195,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -2200,7 +2205,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -2210,7 +2215,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -2220,7 +2225,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -2230,7 +2235,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -2240,7 +2245,7 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -2250,7 +2255,7 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -2260,7 +2265,7 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2270,7 +2275,7 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2280,7 +2285,7 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2290,7 +2295,7 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2300,7 +2305,7 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -2310,7 +2315,7 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -2320,7 +2325,7 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -2330,7 +2335,7 @@
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>

</xml_diff>

<commit_message>
Updated Test Case Summary
</commit_message>
<xml_diff>
--- a/Analysis/Test Cases/System Test Case Summary.xlsx
+++ b/Analysis/Test Cases/System Test Case Summary.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="98">
   <si>
     <t>Title</t>
   </si>
@@ -111,9 +111,6 @@
     <t>Get weekly member service report for a member</t>
   </si>
   <si>
-    <t>Automatically generate weekly EFT data for all providers</t>
-  </si>
-  <si>
     <t>Automatically generate weekly member service reports for all members</t>
   </si>
   <si>
@@ -172,12 +169,6 @@
   </si>
   <si>
     <t>RPRT005</t>
-  </si>
-  <si>
-    <t>RPRT006</t>
-  </si>
-  <si>
-    <t>RPRT007</t>
   </si>
   <si>
     <t>Access to test build</t>
@@ -278,15 +269,6 @@
     <t>The system should be able to generate weekly member service reports for all member. The system will generate the reports as previously scheduled by a user.</t>
   </si>
   <si>
-    <t>User should be able to schedule the day and time when the system should automatically generate weekly EFT data for all providers.</t>
-  </si>
-  <si>
-    <t>Schedule day and time to generate all weekly EFT data for all providers</t>
-  </si>
-  <si>
-    <t>The system should be able to generate weekly EFT data for all providers. The system will generate the data as previously scheduled by a user.</t>
-  </si>
-  <si>
     <t>Show validation status and go back to menu upon success. And on error return back to menu.</t>
   </si>
   <si>
@@ -317,9 +299,6 @@
     <t>Verify weeky service fee</t>
   </si>
   <si>
-    <t>User should be able to verify the wwekly service fee.</t>
-  </si>
-  <si>
     <t>ACTM009</t>
   </si>
   <si>
@@ -344,7 +323,49 @@
     <t>Weekly provider report scheduler's day and time are changed properly. The reports are generated according to the new schedule. Success message is shown.</t>
   </si>
   <si>
-    <t>Show member information</t>
+    <t>Show member information.</t>
+  </si>
+  <si>
+    <t>Member information is added in the system.</t>
+  </si>
+  <si>
+    <t>Provider information is updated in the system. Success message is shown.</t>
+  </si>
+  <si>
+    <t>Service directory is updated in the system. Success message is shown.</t>
+  </si>
+  <si>
+    <t>Member information is removed from the system. Success message is shown.</t>
+  </si>
+  <si>
+    <t>Show provider information. Success message is shown.</t>
+  </si>
+  <si>
+    <t>Provider information is added in the system. Success message is shown.</t>
+  </si>
+  <si>
+    <t>Member status is updated in the system. Success message is shown.</t>
+  </si>
+  <si>
+    <t>Show all service directory. Success message is shown.</t>
+  </si>
+  <si>
+    <t>Service record is added in the system. Success message is shown.</t>
+  </si>
+  <si>
+    <t>User should be able to verify the weekly service fee.</t>
+  </si>
+  <si>
+    <t>The weekly  service fee checklist is marked as "verified" in the system. Success message is shown.</t>
+  </si>
+  <si>
+    <t>The weekly service report should be retreiveable. Success message is shown.</t>
+  </si>
+  <si>
+    <t>Weekly member report scheduler's day and time are changed properly. The reports are generated according to the new schedule. Success message is shown.</t>
+  </si>
+  <si>
+    <t>Weekly member service reports should be generated properly.</t>
   </si>
 </sst>
 </file>
@@ -851,9 +872,9 @@
   <dimension ref="A3:H42"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="6" topLeftCell="A22" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="G8" sqref="G8"/>
+      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -913,7 +934,7 @@
     <row r="7" spans="1:8" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>14</v>
@@ -922,20 +943,20 @@
         <v>17</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="H7" s="1"/>
     </row>
     <row r="8" spans="1:8" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>15</v>
@@ -944,20 +965,20 @@
         <v>16</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="H8" s="1"/>
     </row>
     <row r="9" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>15</v>
@@ -966,18 +987,20 @@
         <v>18</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="1"/>
+        <v>51</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="H9" s="1"/>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>15</v>
@@ -986,20 +1009,20 @@
         <v>19</v>
       </c>
       <c r="E10" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F10" s="1" t="s">
-        <v>55</v>
-      </c>
       <c r="G10" s="1" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>15</v>
@@ -1008,18 +1031,20 @@
         <v>20</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" s="1"/>
+        <v>54</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>87</v>
+      </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>15</v>
@@ -1028,18 +1053,20 @@
         <v>21</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" s="1"/>
+        <v>55</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>88</v>
+      </c>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>15</v>
@@ -1048,18 +1075,20 @@
         <v>22</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G13" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>89</v>
+      </c>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>15</v>
@@ -1068,18 +1097,20 @@
         <v>23</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G14" s="1"/>
+        <v>57</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>15</v>
@@ -1088,60 +1119,64 @@
         <v>24</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G16" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>90</v>
+      </c>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="1"/>
+        <v>70</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>91</v>
+      </c>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>25</v>
@@ -1150,80 +1185,86 @@
         <v>26</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F18" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G18" s="1"/>
+        <v>59</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>92</v>
+      </c>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G19" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="G19" s="1" t="s">
+        <v>86</v>
+      </c>
       <c r="H19" s="1"/>
     </row>
     <row r="20" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="H20" s="1"/>
     </row>
     <row r="21" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>25</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G21" s="1"/>
+        <v>93</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>94</v>
+      </c>
       <c r="H21" s="1"/>
     </row>
     <row r="22" spans="1:8" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>27</v>
@@ -1232,133 +1273,121 @@
         <v>28</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" s="1"/>
+        <v>60</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>95</v>
+      </c>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:8" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G23" s="1"/>
+        <v>61</v>
+      </c>
+      <c r="G23" s="1" t="s">
+        <v>96</v>
+      </c>
       <c r="H23" s="1"/>
     </row>
     <row r="24" spans="1:8" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G24" s="1"/>
+        <v>64</v>
+      </c>
+      <c r="G24" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="H24" s="1"/>
     </row>
     <row r="25" spans="1:8" s="5" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="H25" s="1"/>
     </row>
     <row r="26" spans="1:8" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>27</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G26" s="1"/>
+        <v>63</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>97</v>
+      </c>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
-      <c r="B27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>68</v>
-      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
-      <c r="B28" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>70</v>
-      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>

</xml_diff>

<commit_message>
Updated system test case summary
</commit_message>
<xml_diff>
--- a/Analysis/Test Cases/System Test Case Summary.xlsx
+++ b/Analysis/Test Cases/System Test Case Summary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7670" tabRatio="900"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7665" tabRatio="900"/>
   </bookViews>
   <sheets>
     <sheet name="Authentication" sheetId="1" r:id="rId1"/>
@@ -12,16 +12,16 @@
     <sheet name="Reports" sheetId="14" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Authentication!$A$6:$H$13</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Authentication!$A$6:$H$9</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Reports!$A$1:$H$8</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Transaction Processing'!$A$1:$H$8</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Transaction Processing'!$A$1:$H$3</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="93">
   <si>
     <t>Title</t>
   </si>
@@ -33,9 +33,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>UM.01</t>
   </si>
   <si>
     <t>Module/
@@ -51,12 +48,6 @@
     <t>Test Case Id.</t>
   </si>
   <si>
-    <t>RP.01</t>
-  </si>
-  <si>
-    <t>TP.01</t>
-  </si>
-  <si>
     <t xml:space="preserve">Student Names: </t>
   </si>
   <si>
@@ -178,9 +169,6 @@
   </si>
   <si>
     <t>RPRT007</t>
-  </si>
-  <si>
-    <t>Access to test build</t>
   </si>
   <si>
     <r>
@@ -342,6 +330,27 @@
   </si>
   <si>
     <t>Weekly provider report scheduler's day and time are changed properly. The reports are generated according to the new schedule. Success message is shown.</t>
+  </si>
+  <si>
+    <t>Access to test build, valid member information in the database.</t>
+  </si>
+  <si>
+    <t>Access to test build, valid provider information in the database.</t>
+  </si>
+  <si>
+    <t>Access to test build, valid service information in the database.</t>
+  </si>
+  <si>
+    <t>Access to test build, valid member, provider, and service information in the database.</t>
+  </si>
+  <si>
+    <t>Access to test build, valid provider information and service record in the database.</t>
+  </si>
+  <si>
+    <t>Access to test build. Valid member, provider, and service information. Valid service record.</t>
+  </si>
+  <si>
+    <t>Access to test build. Valid report schedule database.</t>
   </si>
 </sst>
 </file>
@@ -406,7 +415,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -451,11 +460,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -489,6 +511,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -847,49 +872,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H42"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="6" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.26953125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="2"/>
+    <col min="3" max="3" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E3" s="10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F3" s="11"/>
     </row>
-    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B5" s="9"/>
       <c r="C5" s="8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="C6" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>0</v>
@@ -898,7 +923,7 @@
         <v>1</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G6" s="7" t="s">
         <v>2</v>
@@ -907,457 +932,44 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:8" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" s="3" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-    </row>
-    <row r="9" spans="1:8" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-    </row>
-    <row r="10" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="H10" s="1"/>
-    </row>
-    <row r="11" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-    </row>
-    <row r="12" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-    </row>
-    <row r="13" spans="1:8" ht="29" x14ac:dyDescent="0.35">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="G13" s="1"/>
-      <c r="H13" s="1"/>
-    </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F14" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-    </row>
-    <row r="15" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F15" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1" t="s">
-        <v>82</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F16" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-    </row>
-    <row r="17" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-    </row>
-    <row r="18" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F18" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-    </row>
-    <row r="19" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H20" s="1"/>
-    </row>
-    <row r="21" spans="1:8" s="5" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="E21" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F21" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="G21" s="1"/>
-      <c r="H21" s="1"/>
-    </row>
-    <row r="22" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F22" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" s="1"/>
-      <c r="H22" s="1"/>
-    </row>
-    <row r="23" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F23" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="G23" s="1"/>
-      <c r="H23" s="1"/>
-    </row>
-    <row r="24" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F24" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="G24" s="1"/>
-      <c r="H24" s="1"/>
-    </row>
-    <row r="25" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="G25" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="H25" s="1"/>
-    </row>
-    <row r="26" spans="1:8" s="5" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F26" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="G26" s="1"/>
-      <c r="H26" s="1"/>
-    </row>
-    <row r="27" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="G27" s="1"/>
-      <c r="H27" s="1"/>
-    </row>
-    <row r="28" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="4"/>
-      <c r="B28" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="F28" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1367,7 +979,7 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1377,7 +989,7 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1387,7 +999,7 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1397,7 +1009,7 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1407,7 +1019,7 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1417,7 +1029,7 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1427,7 +1039,7 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1437,7 +1049,7 @@
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1447,7 +1059,7 @@
       <c r="G37" s="4"/>
       <c r="H37" s="4"/>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="C38" s="4"/>
@@ -1457,7 +1069,7 @@
       <c r="G38" s="4"/>
       <c r="H38" s="4"/>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1467,7 +1079,7 @@
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1477,7 +1089,7 @@
       <c r="G40" s="4"/>
       <c r="H40" s="4"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -1487,7 +1099,7 @@
       <c r="G41" s="4"/>
       <c r="H41" s="4"/>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -1515,31 +1127,31 @@
     <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:H2"/>
+      <selection pane="bottomLeft" activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.26953125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="2"/>
+    <col min="3" max="3" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="C1" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>0</v>
@@ -1548,7 +1160,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>2</v>
@@ -1557,151 +1169,293 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+        <v>32</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>52</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>50</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>82</v>
+      </c>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>53</v>
+      </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>54</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>55</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+      <c r="B8" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>56</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="4"/>
-      <c r="B12" s="4"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="4"/>
-      <c r="B14" s="4"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" s="5" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1711,7 +1465,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1721,7 +1475,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1731,7 +1485,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1741,7 +1495,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1751,7 +1505,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1761,7 +1515,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1771,7 +1525,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1781,7 +1535,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1791,7 +1545,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1801,7 +1555,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1811,7 +1565,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1821,7 +1575,7 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1831,7 +1585,7 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1841,7 +1595,7 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1851,7 +1605,7 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -1861,7 +1615,7 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -1871,7 +1625,7 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -1881,7 +1635,7 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1891,7 +1645,7 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -1901,7 +1655,7 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -1911,7 +1665,7 @@
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
@@ -1931,34 +1685,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H37"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2:H2"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" style="3" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="33.7265625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="54.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="48.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="30.26953125" style="3" customWidth="1"/>
-    <col min="9" max="16384" width="9.1796875" style="2"/>
+    <col min="3" max="3" width="14.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="54.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="48.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="30.28515625" style="3" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="3" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="7" t="s">
-        <v>8</v>
-      </c>
       <c r="C1" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>0</v>
@@ -1967,7 +1721,7 @@
         <v>1</v>
       </c>
       <c r="F1" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>2</v>
@@ -1976,81 +1730,149 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
+    <row r="2" spans="1:8" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
+        <v>42</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>60</v>
+      </c>
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:8" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
-      <c r="D4" s="1"/>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
+      <c r="B4" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>63</v>
+      </c>
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="B5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>85</v>
+      </c>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
+      <c r="B6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>62</v>
+      </c>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+      <c r="B7" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>64</v>
+      </c>
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
+    <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="12"/>
+      <c r="B8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>66</v>
+      </c>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -2060,7 +1882,7 @@
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
     </row>
-    <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2070,7 +1892,7 @@
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
     </row>
-    <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -2080,7 +1902,7 @@
       <c r="G11" s="4"/>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -2090,7 +1912,7 @@
       <c r="G12" s="4"/>
       <c r="H12" s="4"/>
     </row>
-    <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -2100,7 +1922,7 @@
       <c r="G13" s="4"/>
       <c r="H13" s="4"/>
     </row>
-    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -2110,7 +1932,7 @@
       <c r="G14" s="4"/>
       <c r="H14" s="4"/>
     </row>
-    <row r="15" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -2120,7 +1942,7 @@
       <c r="G15" s="4"/>
       <c r="H15" s="4"/>
     </row>
-    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -2130,7 +1952,7 @@
       <c r="G16" s="4"/>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -2140,7 +1962,7 @@
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
     </row>
-    <row r="18" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -2150,7 +1972,7 @@
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
     </row>
-    <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -2160,7 +1982,7 @@
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
     </row>
-    <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -2170,7 +1992,7 @@
       <c r="G20" s="4"/>
       <c r="H20" s="4"/>
     </row>
-    <row r="21" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -2180,7 +2002,7 @@
       <c r="G21" s="4"/>
       <c r="H21" s="4"/>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -2190,7 +2012,7 @@
       <c r="G22" s="4"/>
       <c r="H22" s="4"/>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -2200,7 +2022,7 @@
       <c r="G23" s="4"/>
       <c r="H23" s="4"/>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -2210,7 +2032,7 @@
       <c r="G24" s="4"/>
       <c r="H24" s="4"/>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -2220,7 +2042,7 @@
       <c r="G25" s="4"/>
       <c r="H25" s="4"/>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -2230,7 +2052,7 @@
       <c r="G26" s="4"/>
       <c r="H26" s="4"/>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -2240,7 +2062,7 @@
       <c r="G27" s="4"/>
       <c r="H27" s="4"/>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -2250,7 +2072,7 @@
       <c r="G28" s="4"/>
       <c r="H28" s="4"/>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -2260,7 +2082,7 @@
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2270,7 +2092,7 @@
       <c r="G30" s="4"/>
       <c r="H30" s="4"/>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2280,7 +2102,7 @@
       <c r="G31" s="4"/>
       <c r="H31" s="4"/>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2290,7 +2112,7 @@
       <c r="G32" s="4"/>
       <c r="H32" s="4"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2300,7 +2122,7 @@
       <c r="G33" s="4"/>
       <c r="H33" s="4"/>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -2310,7 +2132,7 @@
       <c r="G34" s="4"/>
       <c r="H34" s="4"/>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -2320,7 +2142,7 @@
       <c r="G35" s="4"/>
       <c r="H35" s="4"/>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="C36" s="4"/>
@@ -2330,7 +2152,7 @@
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>

</xml_diff>